<commit_message>
Final Update On Data
</commit_message>
<xml_diff>
--- a/Group Project Data.xlsx
+++ b/Group Project Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="47">
   <si>
     <t>Monday</t>
   </si>
@@ -107,27 +107,80 @@
     <t>Arrivals/Hour/Day: 22.1535</t>
   </si>
   <si>
-    <t>Bench Ratio (Y:N)</t>
-  </si>
-  <si>
-    <t>Average Wait:</t>
-  </si>
-  <si>
-    <t>Average Lift:</t>
-  </si>
-  <si>
-    <t>Total Wait:</t>
-  </si>
-  <si>
-    <t>Total Lift:</t>
+    <t>Bench Ratio (Y:N): 12:5</t>
+  </si>
+  <si>
+    <t>Bench Ratio (Y:N): 13:7</t>
+  </si>
+  <si>
+    <t>Bench Ratio (Y:N): 12:16</t>
+  </si>
+  <si>
+    <t>Bench Ratio (Y:N): 28:17</t>
+  </si>
+  <si>
+    <t>Total Wait: 234 min</t>
+  </si>
+  <si>
+    <t>Total Lift: 637 min</t>
+  </si>
+  <si>
+    <t>Average Wait: 7.0909</t>
+  </si>
+  <si>
+    <t>Average Lift: 28.9545</t>
+  </si>
+  <si>
+    <t>Total Wait: 112</t>
+  </si>
+  <si>
+    <t>Average Wait: 4.8700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Lift: 352 </t>
+  </si>
+  <si>
+    <t>Average Lift: 23.4667</t>
+  </si>
+  <si>
+    <t>Total Wait: 156</t>
+  </si>
+  <si>
+    <t>Average Wait: 3.8049</t>
+  </si>
+  <si>
+    <t>Total Lift: 715</t>
+  </si>
+  <si>
+    <t>Average Lift: 22.3438</t>
+  </si>
+  <si>
+    <t>Total Wait: 150</t>
+  </si>
+  <si>
+    <t>Total Lift: 989</t>
+  </si>
+  <si>
+    <t>Average Wait: 3.125</t>
+  </si>
+  <si>
+    <t>Average Lift: 24.1220</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -155,11 +208,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P50"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9:P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44:J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +744,7 @@
         <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
@@ -700,7 +754,7 @@
       </c>
       <c r="K6" s="1"/>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M6" s="1">
         <v>3</v>
@@ -712,7 +766,7 @@
         <v>17</v>
       </c>
       <c r="P6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -724,7 +778,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1">
         <v>13</v>
@@ -736,7 +790,7 @@
         <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I7" s="1">
         <v>6</v>
@@ -746,7 +800,7 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M7" s="1">
         <v>4</v>
@@ -758,7 +812,7 @@
         <v>18</v>
       </c>
       <c r="P7" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -770,7 +824,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -782,7 +836,7 @@
         <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="I8" s="1">
         <v>8</v>
@@ -792,7 +846,7 @@
       </c>
       <c r="K8" s="1"/>
       <c r="L8" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
@@ -804,7 +858,7 @@
         <v>18</v>
       </c>
       <c r="P8" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -816,7 +870,7 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1">
         <v>4</v>
@@ -828,7 +882,7 @@
         <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I9" s="1">
         <v>12</v>
@@ -838,7 +892,7 @@
       </c>
       <c r="K9" s="1"/>
       <c r="L9" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="M9" s="1">
         <v>1</v>
@@ -850,7 +904,7 @@
         <v>17</v>
       </c>
       <c r="P9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -862,7 +916,7 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1">
         <v>7</v>
@@ -874,7 +928,7 @@
         <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="I10" s="1">
         <v>13</v>
@@ -884,7 +938,7 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="M10" s="1">
         <v>4</v>
@@ -896,7 +950,7 @@
         <v>18</v>
       </c>
       <c r="P10" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1521,7 +1575,6 @@
       <c r="F28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="1"/>
       <c r="I28" s="1">
         <v>6</v>
       </c>
@@ -1557,7 +1610,6 @@
       <c r="F29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="1"/>
       <c r="I29" s="1">
         <v>4</v>
       </c>
@@ -1593,7 +1645,6 @@
       <c r="F30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="1"/>
       <c r="I30" s="1">
         <v>3</v>
       </c>
@@ -1763,7 +1814,6 @@
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="1"/>
       <c r="I36" s="1">
         <v>0</v>
       </c>
@@ -1790,7 +1840,6 @@
       <c r="B37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="1"/>
       <c r="I37" s="1">
         <v>0</v>
       </c>
@@ -1811,6 +1860,7 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
       <c r="I38" s="1">
         <v>0</v>
       </c>
@@ -1931,6 +1981,8 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
       <c r="M44" s="1">
         <v>1</v>
       </c>
@@ -2006,6 +2058,10 @@
       <c r="O50" s="1" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="51" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
A better data version
</commit_message>
<xml_diff>
--- a/Group Project Data.xlsx
+++ b/Group Project Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="61">
   <si>
     <t>Monday</t>
   </si>
@@ -119,12 +119,6 @@
     <t>Bench Ratio (Y:N): 28:17</t>
   </si>
   <si>
-    <t>Total Wait: 234 min</t>
-  </si>
-  <si>
-    <t>Total Lift: 637 min</t>
-  </si>
-  <si>
     <t>Average Wait: 7.0909</t>
   </si>
   <si>
@@ -165,6 +159,54 @@
   </si>
   <si>
     <t>Average Lift: 24.1220</t>
+  </si>
+  <si>
+    <t>SUPER TOTAL STUFF</t>
+  </si>
+  <si>
+    <t>Total Arrivals: 154</t>
+  </si>
+  <si>
+    <t>Hours Tracked: 7.7834</t>
+  </si>
+  <si>
+    <t>Arrivals/Hour/Day: 19.7857</t>
+  </si>
+  <si>
+    <t>Bench Ratio(Y/N): 65:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Wait: 234 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Lift: 637 </t>
+  </si>
+  <si>
+    <t>Total Wait:  652</t>
+  </si>
+  <si>
+    <t>Total: Lift: 2693</t>
+  </si>
+  <si>
+    <t>Total Working Out: 147</t>
+  </si>
+  <si>
+    <t>Average Wait: 4.4354</t>
+  </si>
+  <si>
+    <t>Average Lift: 18.3197</t>
+  </si>
+  <si>
+    <t>Average above is based off totals</t>
+  </si>
+  <si>
+    <t>The follow is based off each other</t>
+  </si>
+  <si>
+    <t>Average Wait: 4.7227</t>
+  </si>
+  <si>
+    <t>Average Lift: 24.7218</t>
   </si>
 </sst>
 </file>
@@ -208,12 +250,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44:J44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,12 +564,13 @@
     <col min="13" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,8 +583,11 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -584,8 +636,11 @@
       <c r="P2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -630,8 +685,11 @@
       <c r="P3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -676,8 +734,11 @@
       <c r="P4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -722,8 +783,11 @@
       <c r="P5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>7</v>
       </c>
@@ -768,8 +832,11 @@
       <c r="P6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -778,7 +845,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E7" s="1">
         <v>13</v>
@@ -790,7 +857,7 @@
         <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I7" s="1">
         <v>6</v>
@@ -800,7 +867,7 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M7" s="1">
         <v>4</v>
@@ -812,10 +879,13 @@
         <v>18</v>
       </c>
       <c r="P7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>12</v>
       </c>
@@ -824,7 +894,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -836,7 +906,7 @@
         <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I8" s="1">
         <v>8</v>
@@ -846,22 +916,25 @@
       </c>
       <c r="K8" s="1"/>
       <c r="L8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>17</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
-      <c r="N8" s="1">
-        <v>17</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -882,7 +955,7 @@
         <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I9" s="1">
         <v>12</v>
@@ -892,7 +965,7 @@
       </c>
       <c r="K9" s="1"/>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M9" s="1">
         <v>1</v>
@@ -906,8 +979,11 @@
       <c r="P9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -928,7 +1004,7 @@
         <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" s="1">
         <v>13</v>
@@ -938,7 +1014,7 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M10" s="1">
         <v>4</v>
@@ -952,8 +1028,11 @@
       <c r="P10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -986,8 +1065,9 @@
       <c r="O11" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="3"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -1020,8 +1100,11 @@
       <c r="O12" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1056,8 +1139,11 @@
       <c r="O13" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1088,8 +1174,9 @@
         <v>19</v>
       </c>
       <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1120,8 +1207,11 @@
         <v>49</v>
       </c>
       <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>7</v>
       </c>
@@ -1156,8 +1246,11 @@
       <c r="O16" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>3</v>
       </c>
@@ -1190,8 +1283,9 @@
       <c r="O17" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1228,8 +1322,9 @@
       <c r="O18" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1266,8 +1361,9 @@
       <c r="O19" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>5</v>
       </c>
@@ -1304,8 +1400,9 @@
       <c r="O20" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>5</v>
       </c>
@@ -1338,8 +1435,9 @@
         <v>17</v>
       </c>
       <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1376,8 +1474,9 @@
       <c r="O22" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>5</v>
       </c>
@@ -1413,7 +1512,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1449,7 +1548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -1487,7 +1586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>14</v>
       </c>
@@ -1523,7 +1622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>15</v>
       </c>
@@ -1559,7 +1658,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>4</v>
       </c>
@@ -1594,7 +1693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -1629,7 +1728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -1664,7 +1763,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>13</v>
       </c>
@@ -1693,7 +1792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>10</v>
       </c>
@@ -2065,5 +2164,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Changes to Data and README
</commit_message>
<xml_diff>
--- a/Group Project Data.xlsx
+++ b/Group Project Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Desktop\College\Pitt\4thSemester16Spring\CS1538\SimulationAssignments\SimulationProject\SimulationProject\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Ha\Documents\GitHub\GymSimulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -589,7 +589,7 @@
   <dimension ref="A1:AF501"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3"/>
+      <selection activeCell="AF4" sqref="AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,6 +838,10 @@
         <v>0.11666666666666667</v>
       </c>
       <c r="AE3" s="5"/>
+      <c r="AF3">
+        <f>0.0739*60</f>
+        <v>4.4339999999999993</v>
+      </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="5">

</xml_diff>